<commit_message>
communication between TwinManager and HenshinEndpoint works for executeOperation
</commit_message>
<xml_diff>
--- a/extraction consolidation results_V0_3.xlsx
+++ b/extraction consolidation results_V0_3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\05_Projekte\MDE4DT\mde4dts2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Lehner\Desktop\Repos\Paper\MDE4DTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9873B21C-D2F4-41B0-A469-3350EA9503A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA7CF91A-4D4A-4D38-8BB7-9987893A1EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8D11C759-8767-4256-9E25-90A34587B317}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{8D11C759-8767-4256-9E25-90A34587B317}"/>
   </bookViews>
   <sheets>
     <sheet name="extraction consolidation result" sheetId="1" r:id="rId1"/>
@@ -1260,7 +1260,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1299,18 +1299,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="fill"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Ausgabe" xfId="4" builtinId="21"/>
@@ -1733,36 +1721,34 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="Q1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AA28" sqref="AA28"/>
+      <selection pane="topRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.83984375" customWidth="1"/>
+    <col min="2" max="2" width="16.15625" customWidth="1"/>
+    <col min="3" max="3" width="15.41796875" customWidth="1"/>
+    <col min="4" max="4" width="15.15625" customWidth="1"/>
+    <col min="5" max="5" width="16.41796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
     <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="28" customWidth="1"/>
-    <col min="9" max="9" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="25.41796875" customWidth="1"/>
     <col min="10" max="10" width="38" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="12" width="22.42578125" customWidth="1"/>
-    <col min="13" max="13" width="23.5703125" customWidth="1"/>
+    <col min="11" max="11" width="17.26171875" customWidth="1"/>
+    <col min="12" max="12" width="22.41796875" customWidth="1"/>
+    <col min="13" max="13" width="23.578125" customWidth="1"/>
     <col min="14" max="14" width="20" customWidth="1"/>
     <col min="15" max="15" width="31" customWidth="1"/>
-    <col min="16" max="16" width="41.7109375" customWidth="1"/>
-    <col min="17" max="17" width="20.5703125" customWidth="1"/>
-    <col min="18" max="18" width="30.5703125" customWidth="1"/>
-    <col min="19" max="19" width="38.42578125" customWidth="1"/>
-    <col min="20" max="20" width="23.140625" customWidth="1"/>
-    <col min="21" max="21" width="23.140625" style="16" customWidth="1"/>
-    <col min="22" max="22" width="23.140625" customWidth="1"/>
+    <col min="16" max="16" width="41.68359375" customWidth="1"/>
+    <col min="17" max="17" width="20.578125" customWidth="1"/>
+    <col min="18" max="18" width="30.578125" customWidth="1"/>
+    <col min="19" max="19" width="38.41796875" customWidth="1"/>
+    <col min="20" max="22" width="23.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1823,7 +1809,7 @@
       <c r="T1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="U1" s="8" t="s">
         <v>338</v>
       </c>
       <c r="V1" s="1" t="s">
@@ -1839,20 +1825,20 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" t="s">
         <v>329</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" t="s">
         <v>324</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" t="s">
         <v>330</v>
       </c>
       <c r="F2" t="s">
@@ -1876,7 +1862,7 @@
       <c r="N2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="17" t="s">
+      <c r="O2" t="s">
         <v>315</v>
       </c>
       <c r="P2" t="s">
@@ -1894,7 +1880,7 @@
       <c r="T2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="18" t="s">
+      <c r="U2" t="s">
         <v>339</v>
       </c>
       <c r="W2" s="6" t="s">
@@ -1904,13 +1890,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
       <c r="F3" t="s">
         <v>264</v>
       </c>
@@ -1926,29 +1909,27 @@
       <c r="L3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="O3" s="17"/>
       <c r="Q3" t="s">
         <v>27</v>
       </c>
       <c r="S3" t="s">
         <v>29</v>
       </c>
-      <c r="U3" s="18"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="12" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>292</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" t="s">
         <v>329</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" t="s">
         <v>331</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" t="s">
         <v>330</v>
       </c>
       <c r="F4" t="s">
@@ -1972,7 +1953,7 @@
       <c r="N4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="O4" s="17" t="s">
+      <c r="O4" t="s">
         <v>315</v>
       </c>
       <c r="P4" t="s">
@@ -1990,7 +1971,7 @@
       <c r="T4" s="6" t="s">
         <v>301</v>
       </c>
-      <c r="U4" s="18" t="s">
+      <c r="U4" t="s">
         <v>340</v>
       </c>
       <c r="W4" s="6" t="s">
@@ -2000,13 +1981,10 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
       <c r="H5" t="s">
         <v>37</v>
       </c>
@@ -2019,7 +1997,6 @@
       <c r="L5" t="s">
         <v>44</v>
       </c>
-      <c r="O5" s="17"/>
       <c r="Q5" t="s">
         <v>45</v>
       </c>
@@ -2029,22 +2006,21 @@
       <c r="S5" t="s">
         <v>50</v>
       </c>
-      <c r="U5" s="18"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="11" t="s">
         <v>47</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" t="s">
         <v>332</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" t="s">
         <v>322</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" t="s">
         <v>330</v>
       </c>
       <c r="F6" t="s">
@@ -2062,7 +2038,6 @@
       <c r="L6" t="s">
         <v>52</v>
       </c>
-      <c r="O6" s="17"/>
       <c r="P6" t="s">
         <v>49</v>
       </c>
@@ -2075,7 +2050,6 @@
       <c r="S6" t="s">
         <v>50</v>
       </c>
-      <c r="U6" s="18"/>
       <c r="W6" s="6" t="s">
         <v>31</v>
       </c>
@@ -2083,13 +2057,10 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
       <c r="F7" t="s">
         <v>307</v>
       </c>
@@ -2108,22 +2079,17 @@
       <c r="L7" t="s">
         <v>54</v>
       </c>
-      <c r="O7" s="17"/>
       <c r="Q7" t="s">
         <v>45</v>
       </c>
       <c r="S7" t="s">
         <v>50</v>
       </c>
-      <c r="U7" s="18"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
       <c r="F8" t="s">
         <v>36</v>
       </c>
@@ -2142,7 +2108,7 @@
       <c r="N8" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="O8" s="17" t="s">
+      <c r="O8" t="s">
         <v>316</v>
       </c>
       <c r="P8" t="s">
@@ -2160,7 +2126,7 @@
       <c r="T8" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="U8" s="19" t="s">
+      <c r="U8" s="6" t="s">
         <v>341</v>
       </c>
       <c r="W8" s="6" t="s">
@@ -2170,13 +2136,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
       <c r="F9" t="s">
         <v>56</v>
       </c>
@@ -2195,29 +2158,27 @@
       <c r="L9" t="s">
         <v>62</v>
       </c>
-      <c r="O9" s="17"/>
       <c r="Q9" t="s">
         <v>65</v>
       </c>
       <c r="S9" t="s">
         <v>29</v>
       </c>
-      <c r="U9" s="18"/>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="12" t="s">
         <v>55</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" t="s">
         <v>329</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" t="s">
         <v>331</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" t="s">
         <v>319</v>
       </c>
       <c r="F10" t="s">
@@ -2229,23 +2190,21 @@
       <c r="H10" t="s">
         <v>37</v>
       </c>
-      <c r="O10" s="17"/>
-      <c r="U10" s="18"/>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="11" t="s">
         <v>67</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>290</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" t="s">
         <v>332</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" t="s">
         <v>322</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" t="s">
         <v>330</v>
       </c>
       <c r="F11" t="s">
@@ -2269,7 +2228,7 @@
       <c r="N11" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="O11" s="17" t="s">
+      <c r="O11" t="s">
         <v>337</v>
       </c>
       <c r="P11" t="s">
@@ -2284,18 +2243,14 @@
       <c r="S11" t="s">
         <v>50</v>
       </c>
-      <c r="U11" s="18"/>
       <c r="W11" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
       <c r="H12" t="s">
         <v>48</v>
       </c>
@@ -2308,29 +2263,27 @@
       <c r="L12" t="s">
         <v>298</v>
       </c>
-      <c r="O12" s="17"/>
       <c r="Q12" t="s">
         <v>45</v>
       </c>
       <c r="S12" t="s">
         <v>50</v>
       </c>
-      <c r="U12" s="18"/>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="12" t="s">
         <v>71</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" t="s">
         <v>332</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" t="s">
         <v>322</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" t="s">
         <v>330</v>
       </c>
       <c r="F13" t="s">
@@ -2351,7 +2304,6 @@
       <c r="M13" t="s">
         <v>75</v>
       </c>
-      <c r="O13" s="17"/>
       <c r="P13" t="s">
         <v>76</v>
       </c>
@@ -2367,20 +2319,17 @@
       <c r="T13" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="U13" s="18" t="s">
+      <c r="U13" t="s">
         <v>340</v>
       </c>
       <c r="W13" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
       <c r="H14" t="s">
         <v>48</v>
       </c>
@@ -2393,29 +2342,27 @@
       <c r="L14" t="s">
         <v>80</v>
       </c>
-      <c r="O14" s="17"/>
       <c r="Q14" t="s">
         <v>27</v>
       </c>
       <c r="S14" t="s">
         <v>29</v>
       </c>
-      <c r="U14" s="18"/>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="11" t="s">
         <v>81</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" t="s">
         <v>332</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" t="s">
         <v>322</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" t="s">
         <v>330</v>
       </c>
       <c r="F15" t="s">
@@ -2442,7 +2389,7 @@
       <c r="N15" t="s">
         <v>86</v>
       </c>
-      <c r="O15" s="17" t="s">
+      <c r="O15" t="s">
         <v>315</v>
       </c>
       <c r="P15" t="s">
@@ -2460,7 +2407,7 @@
       <c r="T15" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="U15" s="18" t="s">
+      <c r="U15" t="s">
         <v>340</v>
       </c>
       <c r="W15" t="s">
@@ -2473,13 +2420,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
       <c r="F16" t="s">
         <v>84</v>
       </c>
@@ -2498,29 +2442,27 @@
       <c r="L16" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="O16" s="17"/>
       <c r="Q16" t="s">
         <v>59</v>
       </c>
       <c r="S16" t="s">
         <v>29</v>
       </c>
-      <c r="U16" s="18"/>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="12" t="s">
         <v>259</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" t="s">
         <v>332</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" t="s">
         <v>324</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" t="s">
         <v>330</v>
       </c>
       <c r="F17" t="s">
@@ -2544,7 +2486,7 @@
       <c r="N17" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="O17" s="17" t="s">
+      <c r="O17" t="s">
         <v>318</v>
       </c>
       <c r="P17" t="s">
@@ -2559,18 +2501,14 @@
       <c r="S17" t="s">
         <v>29</v>
       </c>
-      <c r="U17" s="18"/>
       <c r="W17" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
       <c r="G18" t="s">
         <v>283</v>
       </c>
@@ -2586,29 +2524,27 @@
       <c r="L18" t="s">
         <v>98</v>
       </c>
-      <c r="O18" s="17"/>
       <c r="Q18" t="s">
         <v>45</v>
       </c>
       <c r="S18" t="s">
         <v>29</v>
       </c>
-      <c r="U18" s="18"/>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="11" t="s">
         <v>99</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" t="s">
         <v>333</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" t="s">
         <v>322</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" t="s">
         <v>330</v>
       </c>
       <c r="F19" t="s">
@@ -2629,7 +2565,7 @@
       <c r="N19" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="O19" s="17" t="s">
+      <c r="O19" t="s">
         <v>315</v>
       </c>
       <c r="P19" t="s">
@@ -2647,7 +2583,7 @@
       <c r="T19" t="s">
         <v>105</v>
       </c>
-      <c r="U19" s="18" t="s">
+      <c r="U19" t="s">
         <v>342</v>
       </c>
       <c r="W19" s="6" t="s">
@@ -2657,20 +2593,20 @@
         <v>106</v>
       </c>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="12" t="s">
         <v>107</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="5" t="s">
         <v>332</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="5" t="s">
         <v>322</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="5" t="s">
         <v>319</v>
       </c>
       <c r="F20" t="s">
@@ -2691,7 +2627,7 @@
       <c r="N20" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="O20" s="17" t="s">
+      <c r="O20" t="s">
         <v>317</v>
       </c>
       <c r="P20" t="s">
@@ -2709,7 +2645,7 @@
       <c r="T20" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="U20" s="18" t="s">
+      <c r="U20" t="s">
         <v>342</v>
       </c>
       <c r="W20" s="6" t="s">
@@ -2722,46 +2658,36 @@
         <v>115</v>
       </c>
     </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
       <c r="F21" t="s">
         <v>111</v>
       </c>
-      <c r="O21" s="17"/>
-      <c r="U21" s="18"/>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
       <c r="F22" t="s">
         <v>116</v>
       </c>
-      <c r="O22" s="17"/>
-      <c r="U22" s="18"/>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="11" t="s">
         <v>117</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" t="s">
         <v>332</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" t="s">
         <v>322</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" t="s">
         <v>330</v>
       </c>
       <c r="F23" t="s">
@@ -2785,7 +2711,7 @@
       <c r="N23" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="O23" s="17" t="s">
+      <c r="O23" t="s">
         <v>337</v>
       </c>
       <c r="P23" t="s">
@@ -2803,7 +2729,7 @@
       <c r="T23" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="U23" s="19" t="s">
+      <c r="U23" s="6" t="s">
         <v>343</v>
       </c>
       <c r="V23" s="6" t="s">
@@ -2816,13 +2742,10 @@
         <v>124</v>
       </c>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
       <c r="F24" t="s">
         <v>125</v>
       </c>
@@ -2838,22 +2761,17 @@
       <c r="L24" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="O24" s="17"/>
       <c r="Q24" t="s">
         <v>59</v>
       </c>
       <c r="S24" t="s">
         <v>50</v>
       </c>
-      <c r="U24" s="18"/>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
       <c r="F25" t="s">
         <v>261</v>
       </c>
@@ -2869,22 +2787,17 @@
       <c r="L25" t="s">
         <v>129</v>
       </c>
-      <c r="O25" s="17"/>
       <c r="Q25" t="s">
         <v>59</v>
       </c>
       <c r="S25" t="s">
         <v>50</v>
       </c>
-      <c r="U25" s="18"/>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
       <c r="F26" t="s">
         <v>130</v>
       </c>
@@ -2900,22 +2813,17 @@
       <c r="L26" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="O26" s="17"/>
       <c r="Q26" t="s">
         <v>59</v>
       </c>
       <c r="S26" t="s">
         <v>50</v>
       </c>
-      <c r="U26" s="18"/>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
       <c r="F27" t="s">
         <v>260</v>
       </c>
@@ -2931,22 +2839,17 @@
       <c r="L27" t="s">
         <v>134</v>
       </c>
-      <c r="O27" s="17"/>
       <c r="Q27" t="s">
         <v>45</v>
       </c>
       <c r="S27" t="s">
         <v>50</v>
       </c>
-      <c r="U27" s="18"/>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
       <c r="F28" t="s">
         <v>135</v>
       </c>
@@ -2962,22 +2865,17 @@
       <c r="L28" t="s">
         <v>137</v>
       </c>
-      <c r="O28" s="17"/>
       <c r="Q28" t="s">
         <v>45</v>
       </c>
       <c r="S28" t="s">
         <v>50</v>
       </c>
-      <c r="U28" s="18"/>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
       <c r="F29" t="s">
         <v>138</v>
       </c>
@@ -2993,22 +2891,17 @@
       <c r="L29" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="O29" s="17"/>
       <c r="Q29" t="s">
         <v>59</v>
       </c>
       <c r="S29" t="s">
         <v>50</v>
       </c>
-      <c r="U29" s="18"/>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
       <c r="F30" t="s">
         <v>142</v>
       </c>
@@ -3027,7 +2920,6 @@
       <c r="M30" s="6" t="s">
         <v>303</v>
       </c>
-      <c r="O30" s="17"/>
       <c r="P30" t="s">
         <v>144</v>
       </c>
@@ -3043,7 +2935,7 @@
       <c r="T30" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="U30" s="18" t="s">
+      <c r="U30" t="s">
         <v>340</v>
       </c>
       <c r="W30" s="6" t="s">
@@ -3053,13 +2945,10 @@
         <v>146</v>
       </c>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
       <c r="F31" t="s">
         <v>143</v>
       </c>
@@ -3075,22 +2964,17 @@
       <c r="L31" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="O31" s="17"/>
       <c r="Q31" t="s">
         <v>59</v>
       </c>
       <c r="S31" t="s">
         <v>29</v>
       </c>
-      <c r="U31" s="18"/>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
       <c r="H32" t="s">
         <v>37</v>
       </c>
@@ -3103,29 +2987,27 @@
       <c r="L32" t="s">
         <v>148</v>
       </c>
-      <c r="O32" s="17"/>
       <c r="Q32" t="s">
         <v>59</v>
       </c>
       <c r="S32" t="s">
         <v>29</v>
       </c>
-      <c r="U32" s="18"/>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="11" t="s">
         <v>149</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C33" t="s">
         <v>329</v>
       </c>
-      <c r="D33" s="14" t="s">
+      <c r="D33" t="s">
         <v>331</v>
       </c>
-      <c r="E33" s="14" t="s">
+      <c r="E33" t="s">
         <v>330</v>
       </c>
       <c r="F33" t="s">
@@ -3146,7 +3028,7 @@
       <c r="N33" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="O33" s="17" t="s">
+      <c r="O33" t="s">
         <v>318</v>
       </c>
       <c r="P33" t="s">
@@ -3158,7 +3040,6 @@
       <c r="S33" t="s">
         <v>29</v>
       </c>
-      <c r="U33" s="18"/>
       <c r="V33" s="6" t="s">
         <v>154</v>
       </c>
@@ -3169,20 +3050,20 @@
         <v>153</v>
       </c>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="12" t="s">
         <v>155</v>
       </c>
       <c r="B34" s="13" t="s">
         <v>320</v>
       </c>
-      <c r="C34" s="14" t="s">
+      <c r="C34" t="s">
         <v>334</v>
       </c>
-      <c r="D34" s="14" t="s">
+      <c r="D34" t="s">
         <v>331</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" t="s">
         <v>319</v>
       </c>
       <c r="F34" t="s">
@@ -3206,7 +3087,6 @@
       <c r="M34" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="O34" s="17"/>
       <c r="P34" t="s">
         <v>144</v>
       </c>
@@ -3219,7 +3099,6 @@
       <c r="S34" t="s">
         <v>29</v>
       </c>
-      <c r="U34" s="18"/>
       <c r="V34" s="6" t="s">
         <v>158</v>
       </c>
@@ -3227,33 +3106,28 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="12" t="s">
         <v>155</v>
       </c>
-      <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
       <c r="F35" t="s">
         <v>159</v>
       </c>
-      <c r="O35" s="17"/>
-      <c r="U35" s="18"/>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="11" t="s">
         <v>93</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C36" t="s">
         <v>332</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D36" t="s">
         <v>324</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E36" t="s">
         <v>330</v>
       </c>
       <c r="F36" t="s">
@@ -3277,7 +3151,7 @@
       <c r="N36" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="O36" s="17" t="s">
+      <c r="O36" t="s">
         <v>315</v>
       </c>
       <c r="P36" t="s">
@@ -3292,18 +3166,14 @@
       <c r="S36" t="s">
         <v>29</v>
       </c>
-      <c r="U36" s="18"/>
       <c r="W36" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
       <c r="H37" t="s">
         <v>37</v>
       </c>
@@ -3316,22 +3186,17 @@
       <c r="L37" t="s">
         <v>98</v>
       </c>
-      <c r="O37" s="17"/>
       <c r="Q37" t="s">
         <v>45</v>
       </c>
       <c r="S37" t="s">
         <v>29</v>
       </c>
-      <c r="U37" s="18"/>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
       <c r="F38" t="s">
         <v>161</v>
       </c>
@@ -3350,7 +3215,7 @@
       <c r="N38" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="O38" s="17" t="s">
+      <c r="O38" t="s">
         <v>318</v>
       </c>
       <c r="P38" t="s">
@@ -3365,7 +3230,6 @@
       <c r="S38" t="s">
         <v>29</v>
       </c>
-      <c r="U38" s="18"/>
       <c r="W38" s="6" t="s">
         <v>31</v>
       </c>
@@ -3373,13 +3237,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
       <c r="F39" t="s">
         <v>262</v>
       </c>
@@ -3395,45 +3256,38 @@
       <c r="L39" t="s">
         <v>166</v>
       </c>
-      <c r="O39" s="17"/>
       <c r="Q39" t="s">
         <v>59</v>
       </c>
       <c r="S39" t="s">
         <v>29</v>
       </c>
-      <c r="U39" s="18"/>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
       <c r="F40" t="s">
         <v>273</v>
       </c>
       <c r="G40" t="s">
         <v>274</v>
       </c>
-      <c r="O40" s="17"/>
-      <c r="U40" s="18"/>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="11" t="s">
         <v>167</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="C41" s="14" t="s">
+      <c r="C41" t="s">
         <v>335</v>
       </c>
-      <c r="D41" s="14" t="s">
+      <c r="D41" t="s">
         <v>324</v>
       </c>
-      <c r="E41" s="14" t="s">
+      <c r="E41" t="s">
         <v>319</v>
       </c>
       <c r="F41" t="s">
@@ -3451,7 +3305,7 @@
       <c r="N41" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="O41" s="17" t="s">
+      <c r="O41" t="s">
         <v>318</v>
       </c>
       <c r="P41" t="s">
@@ -3466,7 +3320,6 @@
       <c r="S41" t="s">
         <v>50</v>
       </c>
-      <c r="U41" s="18"/>
       <c r="W41" t="s">
         <v>79</v>
       </c>
@@ -3474,36 +3327,31 @@
         <v>171</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
       <c r="F42" t="s">
         <v>275</v>
       </c>
       <c r="G42" t="s">
         <v>268</v>
       </c>
-      <c r="O42" s="17"/>
-      <c r="U42" s="18"/>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="12" t="s">
         <v>172</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C43" s="14" t="s">
+      <c r="C43" t="s">
         <v>336</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D43" t="s">
         <v>322</v>
       </c>
-      <c r="E43" s="14" t="s">
+      <c r="E43" t="s">
         <v>330</v>
       </c>
       <c r="F43" t="s">
@@ -3527,7 +3375,7 @@
       <c r="N43" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="O43" s="17" t="s">
+      <c r="O43" t="s">
         <v>318</v>
       </c>
       <c r="P43" t="s">
@@ -3545,20 +3393,17 @@
       <c r="T43" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="U43" s="18" t="s">
+      <c r="U43" t="s">
         <v>339</v>
       </c>
       <c r="W43" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
       <c r="F44" t="s">
         <v>142</v>
       </c>
@@ -3574,29 +3419,27 @@
       <c r="L44" t="s">
         <v>294</v>
       </c>
-      <c r="O44" s="17"/>
       <c r="Q44" t="s">
         <v>45</v>
       </c>
       <c r="S44" t="s">
         <v>29</v>
       </c>
-      <c r="U44" s="18"/>
-    </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="11" t="s">
         <v>177</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C45" t="s">
         <v>336</v>
       </c>
-      <c r="D45" s="14" t="s">
+      <c r="D45" t="s">
         <v>322</v>
       </c>
-      <c r="E45" s="14" t="s">
+      <c r="E45" t="s">
         <v>330</v>
       </c>
       <c r="F45" t="s">
@@ -3614,7 +3457,6 @@
       <c r="L45" t="s">
         <v>181</v>
       </c>
-      <c r="O45" s="17"/>
       <c r="P45" t="s">
         <v>87</v>
       </c>
@@ -3627,7 +3469,7 @@
       <c r="T45" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="U45" s="19" t="s">
+      <c r="U45" s="6" t="s">
         <v>342</v>
       </c>
       <c r="V45" s="6" t="s">
@@ -3641,13 +3483,10 @@
         <v>automatic fire extinguishing system</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
       <c r="F46" t="s">
         <v>184</v>
       </c>
@@ -3663,7 +3502,6 @@
       <c r="L46" t="s">
         <v>185</v>
       </c>
-      <c r="O46" s="17"/>
       <c r="Q46" t="s">
         <v>59</v>
       </c>
@@ -3673,15 +3511,11 @@
       <c r="S46" t="s">
         <v>29</v>
       </c>
-      <c r="U46" s="18"/>
-    </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
       <c r="F47" t="s">
         <v>186</v>
       </c>
@@ -3697,22 +3531,17 @@
       <c r="L47" t="s">
         <v>187</v>
       </c>
-      <c r="O47" s="17"/>
       <c r="Q47" t="s">
         <v>59</v>
       </c>
       <c r="S47" t="s">
         <v>29</v>
       </c>
-      <c r="U47" s="18"/>
-    </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
       <c r="F48" t="s">
         <v>188</v>
       </c>
@@ -3728,22 +3557,17 @@
       <c r="L48" t="s">
         <v>189</v>
       </c>
-      <c r="O48" s="17"/>
       <c r="Q48" t="s">
         <v>59</v>
       </c>
       <c r="S48" t="s">
         <v>29</v>
       </c>
-      <c r="U48" s="18"/>
-    </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
       <c r="F49" t="s">
         <v>190</v>
       </c>
@@ -3759,29 +3583,27 @@
       <c r="L49" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="O49" s="17"/>
       <c r="Q49" t="s">
         <v>59</v>
       </c>
       <c r="S49" t="s">
         <v>29</v>
       </c>
-      <c r="U49" s="18"/>
-    </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="12" t="s">
         <v>193</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C50" s="14" t="s">
+      <c r="C50" t="s">
         <v>329</v>
       </c>
-      <c r="D50" s="14" t="s">
+      <c r="D50" t="s">
         <v>331</v>
       </c>
-      <c r="E50" s="14" t="s">
+      <c r="E50" t="s">
         <v>319</v>
       </c>
       <c r="F50" t="s">
@@ -3802,7 +3624,7 @@
       <c r="N50" t="s">
         <v>196</v>
       </c>
-      <c r="O50" s="17" t="s">
+      <c r="O50" t="s">
         <v>318</v>
       </c>
       <c r="P50" t="s">
@@ -3817,7 +3639,6 @@
       <c r="S50" t="s">
         <v>29</v>
       </c>
-      <c r="U50" s="18"/>
       <c r="V50" s="6" t="s">
         <v>199</v>
       </c>
@@ -3828,13 +3649,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
       <c r="F51" t="s">
         <v>276</v>
       </c>
@@ -3856,7 +3674,7 @@
       <c r="N51" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="O51" s="17" t="s">
+      <c r="O51" t="s">
         <v>333</v>
       </c>
       <c r="P51" t="s">
@@ -3871,7 +3689,6 @@
       <c r="S51" t="s">
         <v>29</v>
       </c>
-      <c r="U51" s="18"/>
       <c r="W51" s="6" t="s">
         <v>31</v>
       </c>
@@ -3879,13 +3696,10 @@
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
       <c r="H52" t="s">
         <v>48</v>
       </c>
@@ -3898,29 +3712,27 @@
       <c r="L52" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="O52" s="17"/>
       <c r="Q52" t="s">
         <v>27</v>
       </c>
       <c r="S52" t="s">
         <v>29</v>
       </c>
-      <c r="U52" s="18"/>
-    </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="12" t="s">
         <v>207</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>284</v>
       </c>
-      <c r="C53" s="14" t="s">
+      <c r="C53" t="s">
         <v>336</v>
       </c>
-      <c r="D53" s="14" t="s">
+      <c r="D53" t="s">
         <v>322</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="E53" t="s">
         <v>330</v>
       </c>
       <c r="F53" t="s">
@@ -3938,7 +3750,6 @@
       <c r="L53" t="s">
         <v>209</v>
       </c>
-      <c r="O53" s="17"/>
       <c r="P53" t="s">
         <v>26</v>
       </c>
@@ -3951,7 +3762,6 @@
       <c r="S53" t="s">
         <v>29</v>
       </c>
-      <c r="U53" s="18"/>
       <c r="W53" s="6" t="s">
         <v>31</v>
       </c>
@@ -3959,13 +3769,10 @@
         <v>210</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
       <c r="F54" t="s">
         <v>212</v>
       </c>
@@ -3984,7 +3791,7 @@
       <c r="N54" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="O54" s="17" t="s">
+      <c r="O54" t="s">
         <v>315</v>
       </c>
       <c r="P54" t="s">
@@ -3996,7 +3803,6 @@
       <c r="S54" t="s">
         <v>29</v>
       </c>
-      <c r="U54" s="18"/>
       <c r="W54" s="6" t="s">
         <v>31</v>
       </c>
@@ -4004,13 +3810,10 @@
         <v>115</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
       <c r="F55" t="s">
         <v>110</v>
       </c>
@@ -4026,22 +3829,17 @@
       <c r="L55" t="s">
         <v>216</v>
       </c>
-      <c r="O55" s="17"/>
       <c r="Q55" t="s">
         <v>27</v>
       </c>
       <c r="S55" t="s">
         <v>29</v>
       </c>
-      <c r="U55" s="18"/>
-    </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
       <c r="F56" t="s">
         <v>116</v>
       </c>
@@ -4057,22 +3855,17 @@
       <c r="L56" t="s">
         <v>218</v>
       </c>
-      <c r="O56" s="17"/>
       <c r="Q56" t="s">
         <v>27</v>
       </c>
       <c r="S56" t="s">
         <v>29</v>
       </c>
-      <c r="U56" s="18"/>
-    </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
       <c r="F57" t="s">
         <v>278</v>
       </c>
@@ -4091,29 +3884,27 @@
       <c r="L57" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="O57" s="17"/>
       <c r="Q57" t="s">
         <v>27</v>
       </c>
       <c r="S57" t="s">
         <v>29</v>
       </c>
-      <c r="U57" s="18"/>
-    </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="12" t="s">
         <v>221</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="C58" s="14" t="s">
+      <c r="C58" t="s">
         <v>334</v>
       </c>
-      <c r="D58" s="14" t="s">
+      <c r="D58" t="s">
         <v>322</v>
       </c>
-      <c r="E58" s="14" t="s">
+      <c r="E58" t="s">
         <v>330</v>
       </c>
       <c r="F58" t="s">
@@ -4137,7 +3928,7 @@
       <c r="N58" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="O58" s="17" t="s">
+      <c r="O58" t="s">
         <v>315</v>
       </c>
       <c r="P58" t="s">
@@ -4152,7 +3943,6 @@
       <c r="S58" t="s">
         <v>29</v>
       </c>
-      <c r="U58" s="18"/>
       <c r="W58" s="6" t="s">
         <v>31</v>
       </c>
@@ -4160,13 +3950,10 @@
         <v>224</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
       <c r="F59" t="s">
         <v>225</v>
       </c>
@@ -4182,42 +3969,35 @@
       <c r="L59" t="s">
         <v>226</v>
       </c>
-      <c r="O59" s="17"/>
       <c r="Q59" t="s">
         <v>27</v>
       </c>
       <c r="S59" t="s">
         <v>29</v>
       </c>
-      <c r="U59" s="18"/>
-    </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="12" t="s">
         <v>221</v>
       </c>
-      <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
       <c r="F60" t="s">
         <v>142</v>
       </c>
-      <c r="O60" s="17"/>
-      <c r="U60" s="18"/>
-    </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="11" t="s">
         <v>227</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C61" t="s">
         <v>336</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D61" t="s">
         <v>322</v>
       </c>
-      <c r="E61" s="14" t="s">
+      <c r="E61" t="s">
         <v>330</v>
       </c>
       <c r="F61" t="s">
@@ -4235,7 +4015,6 @@
       <c r="L61" t="s">
         <v>228</v>
       </c>
-      <c r="O61" s="17"/>
       <c r="P61" t="s">
         <v>41</v>
       </c>
@@ -4251,20 +4030,17 @@
       <c r="T61" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="U61" s="18" t="s">
+      <c r="U61" t="s">
         <v>339</v>
       </c>
       <c r="W61" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
       <c r="F62" t="s">
         <v>230</v>
       </c>
@@ -4280,22 +4056,17 @@
       <c r="L62" t="s">
         <v>231</v>
       </c>
-      <c r="O62" s="17"/>
       <c r="Q62" t="s">
         <v>59</v>
       </c>
       <c r="S62" t="s">
         <v>29</v>
       </c>
-      <c r="U62" s="18"/>
-    </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="11" t="s">
         <v>227</v>
       </c>
-      <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
       <c r="F63" t="s">
         <v>226</v>
       </c>
@@ -4311,29 +4082,27 @@
       <c r="L63" t="s">
         <v>232</v>
       </c>
-      <c r="O63" s="17"/>
       <c r="Q63" t="s">
         <v>59</v>
       </c>
       <c r="S63" t="s">
         <v>29</v>
       </c>
-      <c r="U63" s="18"/>
-    </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="12" t="s">
         <v>233</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C64" t="s">
         <v>333</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D64" t="s">
         <v>322</v>
       </c>
-      <c r="E64" s="14" t="s">
+      <c r="E64" t="s">
         <v>330</v>
       </c>
       <c r="F64" t="s">
@@ -4357,7 +4126,7 @@
       <c r="N64" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="O64" s="17" t="s">
+      <c r="O64" t="s">
         <v>317</v>
       </c>
       <c r="P64" t="s">
@@ -4372,7 +4141,6 @@
       <c r="S64" t="s">
         <v>326</v>
       </c>
-      <c r="U64" s="18"/>
       <c r="W64" s="6" t="s">
         <v>31</v>
       </c>
@@ -4380,20 +4148,20 @@
         <v>238</v>
       </c>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="11" t="s">
         <v>239</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="C65" s="14" t="s">
+      <c r="C65" t="s">
         <v>333</v>
       </c>
-      <c r="D65" s="14" t="s">
+      <c r="D65" t="s">
         <v>322</v>
       </c>
-      <c r="E65" s="14" t="s">
+      <c r="E65" t="s">
         <v>330</v>
       </c>
       <c r="F65" t="s">
@@ -4417,7 +4185,7 @@
       <c r="N65" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="O65" s="17" t="s">
+      <c r="O65" t="s">
         <v>318</v>
       </c>
       <c r="P65" t="s">
@@ -4432,25 +4200,24 @@
       <c r="S65" t="s">
         <v>29</v>
       </c>
-      <c r="U65" s="18"/>
       <c r="W65" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="12" t="s">
         <v>244</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="C66" s="14" t="s">
+      <c r="C66" t="s">
         <v>336</v>
       </c>
-      <c r="D66" s="14" t="s">
+      <c r="D66" t="s">
         <v>322</v>
       </c>
-      <c r="E66" s="14" t="s">
+      <c r="E66" t="s">
         <v>330</v>
       </c>
       <c r="F66" t="s">
@@ -4474,7 +4241,7 @@
       <c r="N66" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="O66" s="17" t="s">
+      <c r="O66" t="s">
         <v>315</v>
       </c>
       <c r="P66" t="s">
@@ -4489,7 +4256,6 @@
       <c r="S66" t="s">
         <v>50</v>
       </c>
-      <c r="U66" s="18"/>
       <c r="W66" s="6" t="s">
         <v>31</v>
       </c>
@@ -4497,13 +4263,10 @@
         <v>250</v>
       </c>
     </row>
-    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
       <c r="H67" t="s">
         <v>37</v>
       </c>
@@ -4516,29 +4279,27 @@
       <c r="L67" t="s">
         <v>251</v>
       </c>
-      <c r="O67" s="17"/>
       <c r="Q67" t="s">
         <v>59</v>
       </c>
       <c r="S67" t="s">
         <v>50</v>
       </c>
-      <c r="U67" s="18"/>
-    </row>
-    <row r="68" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="11" t="s">
         <v>252</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="C68" s="14" t="s">
+      <c r="C68" t="s">
         <v>329</v>
       </c>
-      <c r="D68" s="14" t="s">
+      <c r="D68" t="s">
         <v>324</v>
       </c>
-      <c r="E68" s="14" t="s">
+      <c r="E68" t="s">
         <v>330</v>
       </c>
       <c r="F68" t="s">
@@ -4562,7 +4323,7 @@
       <c r="N68" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="O68" s="17" t="s">
+      <c r="O68" t="s">
         <v>315</v>
       </c>
       <c r="P68" t="s">
@@ -4574,7 +4335,6 @@
       <c r="S68" t="s">
         <v>29</v>
       </c>
-      <c r="U68" s="18"/>
       <c r="W68" s="6" t="s">
         <v>31</v>
       </c>
@@ -4582,13 +4342,8 @@
         <v>258</v>
       </c>
     </row>
-    <row r="69" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="19"/>
-      <c r="C69" s="21"/>
-      <c r="D69" s="21"/>
-      <c r="E69" s="21"/>
-      <c r="O69" s="21"/>
-      <c r="U69" s="18"/>
+    <row r="69" spans="1:25" ht="23.25" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A69" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>